<commit_message>
Updated Docs & Benchmarks
</commit_message>
<xml_diff>
--- a/Benchmark/Benchmarking.xlsx
+++ b/Benchmark/Benchmarking.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14200" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -208,7 +210,7 @@
                   <c:v>183.365964453</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>214.301</c:v>
+                  <c:v>182.76322082</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -281,11 +283,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2132727288"/>
-        <c:axId val="2132239656"/>
+        <c:axId val="-2142350088"/>
+        <c:axId val="-2142343128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2132727288"/>
+        <c:axId val="-2142350088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -318,7 +320,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132239656"/>
+        <c:crossAx val="-2142343128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -326,7 +328,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132239656"/>
+        <c:axId val="-2142343128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -361,7 +363,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132727288"/>
+        <c:crossAx val="-2142350088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -504,6 +506,375 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Pet Monitoring</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$13:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Nap</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Eat</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Bathroom</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Play</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>45.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cloud</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$7:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>182.232197266</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>182.11353125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>183.365964453</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>182.76322082</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Local</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$7:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.65049804687</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.91302587891</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.091095214839999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.11217203613</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2142831880"/>
+        <c:axId val="-2142837496"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2142831880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>#</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Requests</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2142837496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2142837496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time per Request (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2142831880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -561,6 +932,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -893,8 +1338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -942,7 +1387,7 @@
         <v>18336.596445300002</v>
       </c>
       <c r="E3">
-        <v>214301</v>
+        <v>182763.22081999999</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1001,7 +1446,7 @@
       </c>
       <c r="E8" s="1">
         <f>E3/1000</f>
-        <v>214.30099999999999</v>
+        <v>182.76322081999999</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -1074,4 +1519,44 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>